<commit_message>
Split normdists into 2
</commit_message>
<xml_diff>
--- a/resources/Dates_W21B.xlsx
+++ b/resources/Dates_W21B.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>url</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Univariate EDA</t>
   </si>
   <si>
-    <t>Normal Distributions</t>
-  </si>
-  <si>
     <t>Bivariate EDA - Quantitative</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>UnivEDA</t>
   </si>
   <si>
-    <t>NormalDist</t>
-  </si>
-  <si>
     <t>BEDAQuant</t>
   </si>
   <si>
@@ -213,6 +207,18 @@
   </si>
   <si>
     <t>NO CLASS</t>
+  </si>
+  <si>
+    <t>NormalDist1</t>
+  </si>
+  <si>
+    <t>NormalDist2</t>
+  </si>
+  <si>
+    <t>Normal Distributions - Introduction</t>
+  </si>
+  <si>
+    <t>Normal Distributions - Calculations</t>
   </si>
 </sst>
 </file>
@@ -598,18 +604,18 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -635,10 +641,10 @@
         <v>44263</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -674,7 +680,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -692,7 +698,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -710,7 +716,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -728,7 +734,7 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -743,10 +749,10 @@
         <v>44271</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -761,10 +767,10 @@
         <v>44272</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -779,10 +785,10 @@
         <v>44273</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -797,10 +803,10 @@
         <v>44274</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -815,10 +821,10 @@
         <v>44277</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -833,10 +839,10 @@
         <v>44278</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -851,10 +857,10 @@
         <v>44279</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -869,10 +875,10 @@
         <v>44280</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -887,10 +893,10 @@
         <v>44281</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -905,10 +911,10 @@
         <v>44284</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -923,10 +929,10 @@
         <v>44285</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -941,10 +947,10 @@
         <v>44286</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -959,10 +965,10 @@
         <v>44287</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -977,10 +983,10 @@
         <v>44288</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -995,10 +1001,10 @@
         <v>44291</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1013,10 +1019,10 @@
         <v>44292</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1031,10 +1037,10 @@
         <v>44293</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1049,10 +1055,10 @@
         <v>44294</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1067,10 +1073,10 @@
         <v>44295</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1085,10 +1091,10 @@
         <v>44298</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1103,10 +1109,10 @@
         <v>44299</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1121,10 +1127,10 @@
         <v>44300</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1139,10 +1145,10 @@
         <v>44301</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1157,7 +1163,7 @@
         <v>44302</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1172,7 +1178,7 @@
         <v>44305</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1187,7 +1193,7 @@
         <v>44306</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1202,7 +1208,7 @@
         <v>44307</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1217,7 +1223,7 @@
         <v>44308</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1232,7 +1238,7 @@
         <v>44309</v>
       </c>
       <c r="D36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>